<commit_message>
Beginning differential expression analysis
</commit_message>
<xml_diff>
--- a/Hebeloma RNA quantification and plan.xlsx
+++ b/Hebeloma RNA quantification and plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurabogar/Documents/One Plant One Fungus/Hebeloma/Hebeloma_drydown/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{602B6CD4-3185-D447-A6FC-55701955499D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{D924F7BA-FF30-3149-BBC0-820C79666FFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2220" yWindow="500" windowWidth="27640" windowHeight="15840"/>
+    <workbookView xWindow="10760" yWindow="500" windowWidth="27640" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Hebeloma RNA quantification and" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="123">
   <si>
     <t>Sample Name</t>
   </si>
@@ -1240,10 +1240,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14:F21"/>
+      <selection activeCell="B2" sqref="B2:J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1297,7 +1297,7 @@
         <v>32.19</v>
       </c>
       <c r="F2">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G2">
         <v>2.06</v>
@@ -1311,39 +1311,68 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
         <v>12</v>
       </c>
       <c r="E3">
-        <v>9.42</v>
+        <v>19.72</v>
       </c>
       <c r="F3">
+        <v>15</v>
+      </c>
+      <c r="G3">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="H3">
+        <v>2.09</v>
+      </c>
+      <c r="J3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
         <v>12</v>
       </c>
-      <c r="G3">
-        <v>1.82</v>
-      </c>
-      <c r="H3">
-        <v>0.03</v>
-      </c>
-      <c r="J3" t="s">
-        <v>28</v>
+      <c r="E4">
+        <v>9.6</v>
+      </c>
+      <c r="F4">
+        <v>15</v>
+      </c>
+      <c r="G4">
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="H4">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="J4" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
@@ -1352,27 +1381,56 @@
         <v>12</v>
       </c>
       <c r="E5">
-        <v>19.72</v>
+        <v>27.06</v>
       </c>
       <c r="F5">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G5">
-        <v>2.2400000000000002</v>
+        <v>1.72</v>
       </c>
       <c r="H5">
-        <v>2.09</v>
+        <v>0.98</v>
       </c>
       <c r="J5" t="s">
         <v>13</v>
       </c>
     </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6">
+        <v>14.4</v>
+      </c>
+      <c r="F6">
+        <v>15</v>
+      </c>
+      <c r="G6">
+        <v>1.92</v>
+      </c>
+      <c r="H6">
+        <v>1.07</v>
+      </c>
+      <c r="J6" t="s">
+        <v>18</v>
+      </c>
+    </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
         <v>11</v>
@@ -1381,16 +1439,16 @@
         <v>12</v>
       </c>
       <c r="E7">
-        <v>14.4</v>
+        <v>9.11</v>
       </c>
       <c r="F7">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G7">
-        <v>1.92</v>
+        <v>1.76</v>
       </c>
       <c r="H7">
-        <v>1.07</v>
+        <v>1.51</v>
       </c>
       <c r="J7" t="s">
         <v>18</v>
@@ -1398,10 +1456,10 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
@@ -1410,16 +1468,16 @@
         <v>12</v>
       </c>
       <c r="E8">
-        <v>9.11</v>
+        <v>23.3</v>
       </c>
       <c r="F8">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G8">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="H8">
         <v>1.76</v>
-      </c>
-      <c r="H8">
-        <v>1.51</v>
       </c>
       <c r="J8" t="s">
         <v>18</v>
@@ -1427,10 +1485,10 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
         <v>11</v>
@@ -1439,348 +1497,314 @@
         <v>12</v>
       </c>
       <c r="E9">
-        <v>9.6</v>
+        <v>30.66</v>
       </c>
       <c r="F9">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G9">
-        <v>2.0699999999999998</v>
+        <v>1.96</v>
       </c>
       <c r="H9">
-        <v>1.1100000000000001</v>
+        <v>1.35</v>
       </c>
       <c r="J9" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" t="s">
-        <v>20</v>
+      <c r="A10" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>103</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
+        <v>122</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
       </c>
-      <c r="E10">
-        <v>23.3</v>
+      <c r="E10" s="1">
+        <v>16.920000000000002</v>
       </c>
       <c r="F10">
-        <v>14</v>
-      </c>
-      <c r="G10">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="H10">
-        <v>1.76</v>
+        <v>15</v>
+      </c>
+      <c r="G10" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="H10" s="1">
+        <v>1.65</v>
       </c>
       <c r="J10" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>39</v>
-      </c>
-      <c r="B11" t="s">
-        <v>21</v>
+      <c r="A11" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>106</v>
       </c>
       <c r="C11" t="s">
-        <v>11</v>
+        <v>122</v>
       </c>
       <c r="D11" t="s">
         <v>12</v>
       </c>
-      <c r="E11">
-        <v>30.66</v>
+      <c r="E11" s="1">
+        <v>7.09</v>
       </c>
       <c r="F11">
-        <v>14</v>
-      </c>
-      <c r="G11">
-        <v>1.96</v>
-      </c>
-      <c r="H11">
-        <v>1.35</v>
+        <v>15</v>
+      </c>
+      <c r="G11" s="1">
+        <v>2.9</v>
+      </c>
+      <c r="H11" s="1">
+        <v>1.97</v>
       </c>
       <c r="J11" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B12" t="s">
-        <v>16</v>
+      <c r="A12" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>108</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
+        <v>122</v>
       </c>
       <c r="D12" t="s">
         <v>12</v>
       </c>
-      <c r="E12">
-        <v>27.06</v>
+      <c r="E12" s="1">
+        <v>22.06</v>
       </c>
       <c r="F12">
-        <v>14</v>
-      </c>
-      <c r="G12">
-        <v>1.72</v>
-      </c>
-      <c r="H12">
-        <v>0.98</v>
+        <v>15</v>
+      </c>
+      <c r="G12" s="1">
+        <v>2.16</v>
+      </c>
+      <c r="H12" s="1">
+        <v>1.99</v>
       </c>
       <c r="J12" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>43</v>
-      </c>
-      <c r="B13" t="s">
-        <v>29</v>
+      <c r="A13" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>110</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>122</v>
       </c>
       <c r="D13" t="s">
         <v>12</v>
       </c>
-      <c r="E13">
-        <v>59.78</v>
+      <c r="E13" s="1">
+        <v>26.78</v>
       </c>
       <c r="F13">
-        <v>12</v>
-      </c>
-      <c r="G13">
-        <v>1.5</v>
-      </c>
-      <c r="H13">
-        <v>0.52</v>
+        <v>15</v>
+      </c>
+      <c r="G13" s="1">
+        <v>1.95</v>
+      </c>
+      <c r="H13" s="1">
+        <v>1.48</v>
       </c>
       <c r="J13" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="C14" t="s">
         <v>122</v>
       </c>
+      <c r="D14" t="s">
+        <v>12</v>
+      </c>
       <c r="E14" s="1">
-        <v>16.920000000000002</v>
+        <v>11.84</v>
       </c>
       <c r="F14">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G14" s="1">
-        <v>1.8</v>
+        <v>1.68</v>
       </c>
       <c r="H14" s="1">
-        <v>1.65</v>
+        <v>0.95</v>
       </c>
       <c r="J14" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="C15" t="s">
         <v>122</v>
       </c>
+      <c r="D15" t="s">
+        <v>12</v>
+      </c>
       <c r="E15" s="1">
-        <v>7.09</v>
+        <v>12.09</v>
       </c>
       <c r="F15">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G15" s="1">
-        <v>3.03</v>
+        <v>1.61</v>
       </c>
       <c r="H15" s="1">
-        <v>1.97</v>
+        <v>1.19</v>
       </c>
       <c r="J15" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="C16" t="s">
         <v>122</v>
       </c>
+      <c r="D16" t="s">
+        <v>12</v>
+      </c>
       <c r="E16" s="1">
-        <v>22.06</v>
+        <v>14.94</v>
       </c>
       <c r="F16">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G16" s="1">
-        <v>2.16</v>
+        <v>2.2599999999999998</v>
       </c>
       <c r="H16" s="1">
-        <v>1.99</v>
+        <v>1.42</v>
       </c>
       <c r="J16" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="C17" t="s">
         <v>122</v>
       </c>
+      <c r="D17" t="s">
+        <v>12</v>
+      </c>
       <c r="E17" s="1">
-        <v>26.78</v>
+        <v>9.33</v>
       </c>
       <c r="F17">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G17" s="1">
-        <v>1.95</v>
+        <v>1.86</v>
       </c>
       <c r="H17" s="1">
-        <v>1.48</v>
+        <v>1.39</v>
       </c>
       <c r="J17" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>112</v>
+      <c r="A18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" t="s">
+        <v>26</v>
       </c>
       <c r="C18" t="s">
-        <v>122</v>
-      </c>
-      <c r="E18" s="1">
-        <v>11.84</v>
+        <v>27</v>
+      </c>
+      <c r="D18" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18">
+        <v>9.42</v>
       </c>
       <c r="F18">
-        <v>14</v>
-      </c>
-      <c r="G18" s="1">
-        <v>1.68</v>
-      </c>
-      <c r="H18" s="1">
-        <v>0.95</v>
+        <v>15</v>
+      </c>
+      <c r="G18">
+        <v>1.82</v>
+      </c>
+      <c r="H18">
+        <v>0.03</v>
       </c>
       <c r="J18" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>114</v>
+      <c r="A19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" t="s">
+        <v>29</v>
       </c>
       <c r="C19" t="s">
-        <v>122</v>
-      </c>
-      <c r="E19" s="1">
-        <v>12.09</v>
+        <v>30</v>
+      </c>
+      <c r="D19" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19">
+        <v>59.78</v>
       </c>
       <c r="F19">
-        <v>14</v>
-      </c>
-      <c r="G19" s="1">
-        <v>1.61</v>
-      </c>
-      <c r="H19" s="1">
-        <v>1.19</v>
+        <v>15</v>
+      </c>
+      <c r="G19">
+        <v>1.5</v>
+      </c>
+      <c r="H19">
+        <v>0.52</v>
       </c>
       <c r="J19" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="C20" t="s">
-        <v>122</v>
-      </c>
-      <c r="E20" s="1">
-        <v>14.94</v>
-      </c>
-      <c r="F20">
-        <v>14</v>
-      </c>
-      <c r="G20" s="1">
-        <v>2.2599999999999998</v>
-      </c>
-      <c r="H20" s="1">
-        <v>1.42</v>
-      </c>
-      <c r="J20" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="C21" t="s">
-        <v>122</v>
-      </c>
-      <c r="E21" s="1">
-        <v>9.33</v>
-      </c>
-      <c r="F21">
-        <v>14</v>
-      </c>
-      <c r="G21" s="1">
-        <v>1.86</v>
-      </c>
-      <c r="H21" s="1">
-        <v>1.39</v>
-      </c>
-      <c r="J21" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J12">
-    <sortCondition ref="A2:A12"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J21">
+    <sortCondition ref="J2:J21"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>